<commit_message>
Initial commit with all project files
</commit_message>
<xml_diff>
--- a/Template/test.xlsx
+++ b/Template/test.xlsx
@@ -94,76 +94,76 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="20"/>
       <color theme="0"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF111C2F"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF111C2F"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF111C2F"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Audrey"/>
-      <family val="3"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -257,10 +257,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -272,7 +281,10 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -281,6 +293,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="4" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -305,7 +320,9 @@
     <xf numFmtId="4" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -319,24 +336,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -622,256 +621,256 @@
   <dimension ref="A2:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:N3"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" style="17" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" style="17" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="23" style="17" customWidth="1"/>
-    <col min="5" max="5" width="29.1796875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="36.81640625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="20.36328125" style="17" customWidth="1"/>
-    <col min="8" max="8" width="39.1796875" style="17" customWidth="1"/>
-    <col min="9" max="9" width="13.36328125" style="17" customWidth="1"/>
-    <col min="10" max="10" width="13" style="17" customWidth="1"/>
-    <col min="11" max="11" width="15.81640625" style="17" customWidth="1"/>
-    <col min="12" max="12" width="14.453125" style="17" customWidth="1"/>
-    <col min="13" max="13" width="18.36328125" style="17" customWidth="1"/>
-    <col min="14" max="14" width="17.453125" style="17" customWidth="1"/>
-    <col min="15" max="15" width="3.81640625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.6328125" style="1"/>
+    <col min="1" max="1" width="15" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23" style="2" customWidth="1"/>
+    <col min="5" max="5" width="29.1796875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.81640625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="20.36328125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25.7265625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="13.36328125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="13" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.81640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="14.453125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.36328125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="17.453125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="3.81640625" style="2" customWidth="1"/>
+    <col min="16" max="16384" width="8.6328125" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-    </row>
-    <row r="3" spans="1:14" ht="27" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+    </row>
+    <row r="3" spans="1:14" ht="24.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="29"/>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-    </row>
-    <row r="4" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-    </row>
-    <row r="5" spans="1:14" ht="24.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-    </row>
-    <row r="6" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-    </row>
-    <row r="7" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="3" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14" ht="20" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+    </row>
+    <row r="5" spans="1:14" ht="22" x14ac:dyDescent="0.3">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" ht="20" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="20" x14ac:dyDescent="0.3">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="7">
         <f>SUM(N10:N1048576)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="22" x14ac:dyDescent="0.35">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-    </row>
-    <row r="9" spans="1:14" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.35">
-      <c r="A9" s="5" t="s">
+    <row r="8" spans="1:14" ht="20" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" s="10" customFormat="1" ht="17.5" x14ac:dyDescent="0.3">
+      <c r="A9" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="5" t="s">
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="M9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="7"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="11">
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="16">
         <f>ROUND(I10*K10,2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="12"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="14"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="15"/>
-      <c r="N11" s="16"/>
-    </row>
-    <row r="13" spans="1:14" ht="19" x14ac:dyDescent="0.5">
-      <c r="B13" s="28" t="s">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+    </row>
+    <row r="13" spans="1:14" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="28" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="22"/>
+      <c r="F13" s="22"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="19"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
-      <c r="B15" s="20"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="22"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="21"/>
-      <c r="M15" s="22"/>
+      <c r="I13" s="22"/>
+      <c r="J13" s="22"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="22"/>
+      <c r="N13" s="24"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="25"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="27"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="26"/>
+      <c r="J15" s="26"/>
+      <c r="K15" s="26"/>
+      <c r="L15" s="26"/>
+      <c r="M15" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -892,5 +891,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>